<commit_message>
Aggiunti volumi dei dati e frequenze delle operazioni
</commit_message>
<xml_diff>
--- a/doc/Volume dei dati.xlsx
+++ b/doc/Volume dei dati.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Dati</t>
   </si>
@@ -21,49 +21,97 @@
     <t>ToT</t>
   </si>
   <si>
+    <t>Operazioni</t>
+  </si>
+  <si>
+    <t>Volte</t>
+  </si>
+  <si>
+    <t>Tempo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Utente per asta</t>
   </si>
   <si>
     <t>Utenti</t>
   </si>
   <si>
+    <t xml:space="preserve">Registrazione utente</t>
+  </si>
+  <si>
+    <t>mese</t>
+  </si>
+  <si>
     <t xml:space="preserve">Offerte di un utente per un oggetto</t>
   </si>
   <si>
     <t xml:space="preserve">Carta di Credito</t>
   </si>
   <si>
+    <t xml:space="preserve">Visualizza oggetti venduti</t>
+  </si>
+  <si>
+    <t>settimana</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oggetti totali</t>
   </si>
   <si>
     <t>Offerte</t>
   </si>
   <si>
+    <t xml:space="preserve">Visualizza aste in corso</t>
+  </si>
+  <si>
     <t xml:space="preserve">Asta in corso per un utente </t>
   </si>
   <si>
     <t>Controfferte</t>
   </si>
   <si>
+    <t xml:space="preserve">Fai offerta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aste a cui ha partecipato un utente</t>
   </si>
   <si>
     <t>Aste</t>
   </si>
   <si>
+    <t xml:space="preserve">Visualizza oggetti all’asta</t>
+  </si>
+  <si>
+    <t>giorno</t>
+  </si>
+  <si>
     <t xml:space="preserve">Aste in corso</t>
   </si>
   <si>
     <t>Oggetto</t>
   </si>
   <si>
+    <t xml:space="preserve">Inserisci oggetto</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oggetto Venduto</t>
   </si>
   <si>
+    <t xml:space="preserve">Indici asta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oggetto all'asta</t>
   </si>
   <si>
+    <t xml:space="preserve">Inserisci categoria</t>
+  </si>
+  <si>
+    <t>anno</t>
+  </si>
+  <si>
     <t>Possiede</t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
   <si>
     <t>Fa</t>
@@ -85,12 +133,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
       <sz val="11.000000"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.000000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,7 +153,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,12 +161,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,6 +701,9 @@
     <col bestFit="1" min="1" max="1" width="30.7109375"/>
     <col bestFit="1" min="4" max="4" width="15.57421875"/>
     <col bestFit="1" customWidth="1" min="5" max="5" width="11.7109375"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" width="25.19140625"/>
+    <col bestFit="1" min="8" max="8" width="15.140625"/>
+    <col customWidth="1" min="9" max="9" width="16.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -640,129 +713,225 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" ht="14.25">
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" ht="15">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <f>B2*E6</f>
         <v>10000</v>
       </c>
-    </row>
-    <row r="3" ht="14.25">
+      <c r="G2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" ht="15">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E3">
         <f>E2</f>
         <v>10000</v>
       </c>
-    </row>
-    <row r="4" ht="14.25">
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3">
+        <f>H8</f>
+        <v>4000</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" ht="15">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <f>POWER(10,5)</f>
         <v>100000</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <f>E2*B3*B6</f>
         <v>10000000</v>
       </c>
-    </row>
-    <row r="5" ht="14.25">
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <f>2*B5*E2</f>
+        <v>200000</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="15">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <f>E4*0.01</f>
         <v>100000</v>
       </c>
-    </row>
-    <row r="6" ht="14.25">
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5">
+        <f>B3*H10*B5</f>
+        <v>100000</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="15">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E6">
         <f>E9</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="7" ht="14.25">
+      <c r="G6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6">
+        <f>H5</f>
+        <v>100000</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" ht="15">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <f>B4*0.01</f>
         <v>1000</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E7">
         <f>B4</f>
         <v>100000</v>
       </c>
-    </row>
-    <row r="8" ht="14.25">
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <f>4*E6</f>
+        <v>4000</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" ht="15">
       <c r="D8" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E8">
         <f>E7-E9</f>
         <v>99000</v>
       </c>
-    </row>
-    <row r="9" ht="14.25">
+      <c r="G8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8">
+        <f>H7</f>
+        <v>4000</v>
+      </c>
+      <c r="I8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" ht="15">
       <c r="D9" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E9">
         <f>B7</f>
         <v>1000</v>
       </c>
-    </row>
-    <row r="10" ht="14.25">
+      <c r="G9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" ht="15">
       <c r="D10" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="E10">
         <f>E2</f>
         <v>10000</v>
       </c>
-    </row>
-    <row r="11" ht="14.25">
+      <c r="G10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10">
+        <v>1000</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" ht="15">
       <c r="D11" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E11">
         <f>E4</f>
@@ -771,7 +940,7 @@
     </row>
     <row r="12" ht="14.25">
       <c r="D12" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="E12">
         <f>E6*B3*E2/E6</f>
@@ -780,7 +949,7 @@
     </row>
     <row r="13" ht="14.25">
       <c r="D13" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E13">
         <f>E6</f>
@@ -789,20 +958,20 @@
     </row>
     <row r="14" ht="14.25">
       <c r="D14" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E14">
         <f>E4-E12</f>
         <v>9900000</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aggiunta frequenza di 'Disiscrizione Utente'
</commit_message>
<xml_diff>
--- a/doc/Volume dei dati.xlsx
+++ b/doc/Volume dei dati.xlsx
@@ -81,9 +81,6 @@
     <t xml:space="preserve">Visualizza oggetti all’asta</t>
   </si>
   <si>
-    <t>giorno</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aste in corso</t>
   </si>
   <si>
@@ -111,10 +108,13 @@
     <t>Possiede</t>
   </si>
   <si>
+    <t xml:space="preserve">Disiscrizione Utente</t>
+  </si>
+  <si>
+    <t>Fa</t>
+  </si>
+  <si>
     <t>Login</t>
-  </si>
-  <si>
-    <t>Fa</t>
   </si>
   <si>
     <t xml:space="preserve">Viene Fatta</t>
@@ -765,7 +765,7 @@
         <v>11</v>
       </c>
       <c r="H3">
-        <f>H8</f>
+        <f>H7</f>
         <v>4000</v>
       </c>
       <c r="I3" t="s">
@@ -791,8 +791,8 @@
         <v>15</v>
       </c>
       <c r="H4">
-        <f>2*B5*E2</f>
-        <v>200000</v>
+        <f>H11*B5*B3</f>
+        <v>100000</v>
       </c>
       <c r="I4" t="s">
         <v>12</v>
@@ -816,7 +816,7 @@
         <v>18</v>
       </c>
       <c r="H5">
-        <f>B3*H10*B5</f>
+        <f>B3*H11*B5</f>
         <v>100000</v>
       </c>
       <c r="I5" t="s">
@@ -841,30 +841,30 @@
         <v>21</v>
       </c>
       <c r="H6">
-        <f>H5</f>
-        <v>100000</v>
+        <f>H11</f>
+        <v>1000</v>
       </c>
       <c r="I6" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" ht="15">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <f>B4*0.01</f>
         <v>1000</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7">
         <f>B4</f>
         <v>100000</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7">
         <f>4*E6</f>
@@ -876,14 +876,14 @@
     </row>
     <row r="8" ht="15">
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8">
         <f>E7-E9</f>
         <v>99000</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8">
         <f>H7</f>
@@ -895,48 +895,58 @@
     </row>
     <row r="9" ht="15">
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9">
         <f>B7</f>
         <v>1000</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9">
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" ht="15">
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <f>E2</f>
         <v>10000</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>32</v>
+      <c r="G10" t="s">
+        <v>31</v>
       </c>
       <c r="H10">
-        <v>1000</v>
+        <f>H2</f>
+        <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" ht="15">
       <c r="D11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11">
         <f>E4</f>
         <v>10000000</v>
       </c>
+      <c r="G11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11">
+        <v>1000</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" ht="14.25">
       <c r="D12" t="s">
@@ -966,6 +976,11 @@
       </c>
       <c r="F14" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="I20">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring Volume dei dati, Operazioni, Frequenze delle stesse e Calcolo dei costi delle operazioni
</commit_message>
<xml_diff>
--- a/doc/Volume dei dati.xlsx
+++ b/doc/Volume dei dati.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Dati</t>
   </si>
@@ -57,43 +57,37 @@
     <t xml:space="preserve">Carta di Credito</t>
   </si>
   <si>
-    <t xml:space="preserve">Visualizza oggetti venduti</t>
+    <t xml:space="preserve">Visualizza lo stato delle aste dell'utente</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asta in corso per un utente </t>
+  </si>
+  <si>
+    <t>Offerte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fai offerta</t>
   </si>
   <si>
     <t>settimana</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oggetti totali</t>
-  </si>
-  <si>
-    <t>Offerte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visualizza stato asta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asta in corso per un utente </t>
+    <t xml:space="preserve">Aste in corso</t>
   </si>
   <si>
     <t>Controfferte</t>
   </si>
   <si>
-    <t xml:space="preserve">Fai offerta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aste a cui ha partecipato un utente</t>
+    <t xml:space="preserve">Visualizza nuove aste</t>
   </si>
   <si>
     <t>Aste</t>
   </si>
   <si>
-    <t xml:space="preserve">Visualizza nuove aste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aste in corso</t>
+    <t xml:space="preserve">Controfferta Automatica</t>
   </si>
   <si>
     <t>Oggetto</t>
@@ -102,40 +96,28 @@
     <t xml:space="preserve">Inserisci oggetto</t>
   </si>
   <si>
-    <t xml:space="preserve">Possibilie accorpamento con quella sotto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oggetto Venduto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indici asta</t>
+    <t xml:space="preserve">Oggetto Aggiudicato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserisci categoria</t>
+  </si>
+  <si>
+    <t>anno</t>
   </si>
   <si>
     <t xml:space="preserve">Oggetto all'asta</t>
   </si>
   <si>
-    <t xml:space="preserve">Inserisci categoria</t>
-  </si>
-  <si>
-    <t>anno</t>
+    <t>Login</t>
   </si>
   <si>
     <t>Possiede</t>
   </si>
   <si>
-    <t xml:space="preserve">Disiscrizione Utente</t>
-  </si>
-  <si>
     <t>Fa</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t xml:space="preserve">Viene Fatta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Controfferta Automatica</t>
   </si>
   <si>
     <t xml:space="preserve">Viene Messo</t>
@@ -154,16 +136,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
       <sz val="11.000000"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <sz val="12.000000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,7 +152,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -182,33 +160,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,16 +673,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" min="1" max="1" width="30.7109375"/>
-    <col bestFit="1" min="4" max="4" width="15.57421875"/>
+    <col bestFit="1" min="4" max="4" width="18.00390625"/>
     <col bestFit="1" customWidth="1" min="5" max="5" width="11.7109375"/>
-    <col bestFit="1" customWidth="1" min="7" max="7" width="25.19140625"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" width="33.87109375"/>
     <col bestFit="1" min="8" max="8" width="15.140625"/>
     <col customWidth="1" min="9" max="9" width="16.140625"/>
     <col customWidth="1" min="10" max="11" width="18.28125"/>
@@ -766,10 +723,10 @@
         <v>8</v>
       </c>
       <c r="E2">
-        <f>B2*E6</f>
+        <f>10000</f>
         <v>10000</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
       <c r="H2">
@@ -782,8 +739,8 @@
         <v>11</v>
       </c>
       <c r="K2">
-        <f>IF(J2="S",2,1)*(E2+E3+E10)*H2</f>
-        <v>600000</v>
+        <f>IF(J2="S",2,1)*3*H2</f>
+        <v>60</v>
       </c>
     </row>
     <row r="3" ht="15">
@@ -800,56 +757,55 @@
         <f>E2</f>
         <v>10000</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>14</v>
       </c>
       <c r="H3">
-        <f>H7</f>
-        <v>4000</v>
-      </c>
-      <c r="I3" t="s">
+        <f>H4</f>
+        <v>50000</v>
+      </c>
+      <c r="I3" t="str">
+        <f>I4</f>
+        <v>settimana</v>
+      </c>
+      <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
       <c r="K3">
-        <f>IF(J3="S",2,1)*H3*E8</f>
-        <v>396000000</v>
+        <f>IF(J3="S",2,1)*H3*E6</f>
+        <v>5000000</v>
       </c>
     </row>
     <row r="4" ht="15">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="B4">
-        <f>POWER(10,5)</f>
-        <v>100000</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4">
+        <f>E11</f>
+        <v>100000000</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="E4">
-        <f>E2*B3*B6</f>
-        <v>10000000</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4">
+        <f>B3*H9*B4</f>
+        <v>50000</v>
+      </c>
+      <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="H4">
-        <f>H5</f>
-        <v>100000</v>
-      </c>
-      <c r="I4" t="str">
-        <f>I5</f>
-        <v>settimana</v>
-      </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="K4">
-        <f>IF(J4="S",2,1)*H4*E6</f>
-        <v>100000000</v>
+        <f>IF(J4="S",2,1)*H4*E4</f>
+        <v>10000000000000</v>
       </c>
     </row>
     <row r="5" ht="15">
@@ -857,257 +813,190 @@
         <v>20</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <f>100</f>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
       <c r="E5">
         <f>E4*0.01</f>
+        <v>1000000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5">
+        <f>H9</f>
+        <v>1000</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5">
+        <f>IF(J5="S",2,1)*H5*E6</f>
         <v>100000</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5">
-        <f>B3*H11*B5</f>
-        <v>100000</v>
-      </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" t="s">
+    </row>
+    <row r="6" ht="15">
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <f>B5</f>
+        <v>100</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6">
+        <f>H4*0.01</f>
+        <v>500</v>
+      </c>
+      <c r="I6" t="str">
+        <f>I4</f>
+        <v>settimana</v>
+      </c>
+      <c r="J6" t="s">
         <v>11</v>
       </c>
-      <c r="K5">
-        <f>IF(J5="S",2,1)*H5*E4</f>
-        <v>2000000000000</v>
-      </c>
-    </row>
-    <row r="6" ht="15">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6">
-        <v>100</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6">
-        <f>E9</f>
-        <v>1000</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="K6">
+        <f>IF(J6="S",2,1)*H6*E5</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="7" ht="15">
+      <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="H6">
-        <f>H11</f>
-        <v>1000</v>
-      </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6">
-        <f>IF(J6="S",2,1)*H6*E6</f>
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="7" ht="15">
-      <c r="A7" t="s">
+      <c r="E7">
+        <v>10000</v>
+      </c>
+      <c r="G7" t="s">
         <v>26</v>
-      </c>
-      <c r="B7">
-        <f>B4*0.01</f>
-        <v>1000</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7">
-        <f>B4</f>
-        <v>100000</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="H7">
         <f>4*E6</f>
-        <v>4000</v>
+        <v>400</v>
       </c>
       <c r="I7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
         <v>11</v>
       </c>
       <c r="K7">
         <f>IF(J7="S",2,1)*H7*E7</f>
-        <v>800000000</v>
-      </c>
-      <c r="L7" t="s">
-        <v>29</v>
+        <v>8000000</v>
       </c>
     </row>
     <row r="8" ht="15">
       <c r="D8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E8">
         <f>E7-E9</f>
-        <v>99000</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>31</v>
+        <v>9900</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
       </c>
       <c r="H8">
-        <f>H7</f>
-        <v>4000</v>
+        <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="J8" t="s">
         <v>11</v>
       </c>
       <c r="K8">
-        <f>IF(J8="S",2,1)*H8*2</f>
-        <v>16000</v>
+        <f>IF(J8="S",2,1)*H8*E15</f>
+        <v>200</v>
       </c>
     </row>
     <row r="9" ht="15">
       <c r="D9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E9">
-        <f>B7</f>
+        <f>E6</f>
+        <v>100</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9">
         <v>1000</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9">
-        <v>10</v>
-      </c>
       <c r="I9" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="K9">
-        <f>IF(J9="S",2,1)*H9*E15</f>
-        <v>20000</v>
+        <f>IF(J9="S",2,1)*H9</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="10" ht="15">
       <c r="D10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E10">
         <f>E2</f>
         <v>10000</v>
       </c>
-      <c r="G10" t="s">
-        <v>36</v>
-      </c>
-      <c r="H10">
-        <f>H2</f>
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="2">
-        <f>IF(J10="S",2,1)*(E2+E3+E10)*H10</f>
-        <v>600000</v>
-      </c>
     </row>
     <row r="11" ht="15">
       <c r="D11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E11">
-        <f>E4</f>
-        <v>10000000</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H11">
-        <v>1000</v>
-      </c>
-      <c r="I11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11">
-        <f>IF(J11="S",2,1)*H11</f>
-        <v>1000</v>
+        <f>E14+E12</f>
+        <v>100000000</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="D12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E12">
-        <f>E6*B3*E2/E6</f>
-        <v>100000</v>
-      </c>
-      <c r="G12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12">
-        <f>H5*0.01</f>
-        <v>1000</v>
-      </c>
-      <c r="I12" t="str">
-        <f>I5</f>
-        <v>settimana</v>
-      </c>
-      <c r="J12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12">
-        <f>IF(J12="S",2,1)*H12*E5</f>
-        <v>200000000</v>
+        <f>B3*E2*E6/B2</f>
+        <v>1000000</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="D13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E13">
         <f>E6</f>
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="D14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E14">
-        <f>E4-E12</f>
-        <v>9900000</v>
+        <f>B3*E2*E8/B2</f>
+        <v>99000000</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="D15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E15">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" ht="14.25">

</xml_diff>

<commit_message>
Correzzione costo operazione 'Controfferta Automatica'
</commit_message>
<xml_diff>
--- a/doc/Volume dei dati.xlsx
+++ b/doc/Volume dei dati.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Dati</t>
   </si>
@@ -30,12 +30,12 @@
     <t>Tempo</t>
   </si>
   <si>
-    <t>Tipo</t>
-  </si>
-  <si>
     <t>Costo</t>
   </si>
   <si>
+    <t>Note</t>
+  </si>
+  <si>
     <t xml:space="preserve">Utente per asta</t>
   </si>
   <si>
@@ -48,7 +48,7 @@
     <t>mese</t>
   </si>
   <si>
-    <t>S</t>
+    <t>Supposizione</t>
   </si>
   <si>
     <t xml:space="preserve">Offerte di un utente per un oggetto</t>
@@ -60,7 +60,7 @@
     <t xml:space="preserve">Visualizza lo stato delle aste dell'utente</t>
   </si>
   <si>
-    <t>L</t>
+    <t>settimana</t>
   </si>
   <si>
     <t xml:space="preserve">Asta in corso per un utente </t>
@@ -72,9 +72,6 @@
     <t xml:space="preserve">Fai offerta</t>
   </si>
   <si>
-    <t>settimana</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aste in corso</t>
   </si>
   <si>
@@ -84,18 +81,33 @@
     <t xml:space="preserve">Visualizza nuove aste</t>
   </si>
   <si>
+    <t xml:space="preserve">Magari non lo calcolo perché è UNA MERDA DA CALCOLARE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login a settimana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10% degli utenti</t>
+  </si>
+  <si>
     <t>Aste</t>
   </si>
   <si>
     <t xml:space="preserve">Controfferta Automatica</t>
   </si>
   <si>
+    <t xml:space="preserve">1% delle offerte</t>
+  </si>
+  <si>
     <t>Oggetto</t>
   </si>
   <si>
     <t xml:space="preserve">Inserisci oggetto</t>
   </si>
   <si>
+    <t xml:space="preserve"> Numero di volte che un utente visualizza lo stato delle aste al giorno</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oggetto Aggiudicato</t>
   </si>
   <si>
@@ -105,13 +117,22 @@
     <t>anno</t>
   </si>
   <si>
+    <t xml:space="preserve">Visualizza nuove aste per utente a login</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oggetto all'asta</t>
   </si>
   <si>
     <t>Login</t>
   </si>
   <si>
+    <t xml:space="preserve">Durata media asta</t>
+  </si>
+  <si>
     <t>Possiede</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login di un utente a settimana</t>
   </si>
   <si>
     <t>Fa</t>
@@ -164,8 +185,11 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,19 +697,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="30.7109375"/>
+    <col bestFit="1" min="1" max="1" width="58.98046875"/>
+    <col bestFit="1" min="2" max="2" width="14.390625"/>
     <col bestFit="1" min="4" max="4" width="18.00390625"/>
     <col bestFit="1" customWidth="1" min="5" max="5" width="11.7109375"/>
     <col bestFit="1" customWidth="1" min="7" max="7" width="33.87109375"/>
     <col bestFit="1" min="8" max="8" width="15.140625"/>
     <col customWidth="1" min="9" max="9" width="16.140625"/>
-    <col customWidth="1" min="10" max="11" width="18.28125"/>
+    <col customWidth="1" min="10" max="10" width="18.28125"/>
+    <col bestFit="1" customWidth="1" min="11" max="11" width="51.54296875"/>
     <col bestFit="1" min="12" max="12" width="35.00390625"/>
   </cols>
   <sheetData>
@@ -735,12 +761,12 @@
       <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2">
+        <f>2*3*H2</f>
+        <v>60</v>
+      </c>
+      <c r="K2" t="s">
         <v>11</v>
-      </c>
-      <c r="K2">
-        <f>IF(J2="S",2,1)*3*H2</f>
-        <v>60</v>
       </c>
     </row>
     <row r="3" ht="15">
@@ -761,19 +787,15 @@
         <v>14</v>
       </c>
       <c r="H3">
-        <f>H4</f>
-        <v>50000</v>
-      </c>
-      <c r="I3" t="str">
-        <f>I4</f>
-        <v>settimana</v>
-      </c>
-      <c r="J3" t="s">
+        <f>H9</f>
+        <v>4000</v>
+      </c>
+      <c r="I3" t="s">
         <v>15</v>
       </c>
-      <c r="K3">
-        <f>IF(J3="S",2,1)*H3*E6</f>
-        <v>5000000</v>
+      <c r="J3">
+        <f>H3*(1+B2*B4+B4+E14/E12*5)</f>
+        <v>2204000</v>
       </c>
     </row>
     <row r="4" ht="15">
@@ -788,164 +810,183 @@
       </c>
       <c r="E4">
         <f>E11</f>
-        <v>100000000</v>
+        <v>1000000</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
       </c>
       <c r="H4">
-        <f>B3*H9*B4</f>
-        <v>50000</v>
+        <f>E12*B3</f>
+        <v>100000</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4">
-        <f>IF(J4="S",2,1)*H4*E4</f>
-        <v>10000000000000</v>
+        <v>15</v>
+      </c>
+      <c r="J4">
+        <f>2*H4*3</f>
+        <v>600000</v>
       </c>
     </row>
     <row r="5" ht="15">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <f>100</f>
         <v>100</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <f>E4*0.01</f>
-        <v>1000000</v>
+        <v>10000</v>
       </c>
       <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5">
+        <f>H9*B9*B11</f>
+        <v>16000</v>
+      </c>
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5">
+        <f>H5*(E6)</f>
+        <v>1600000</v>
+      </c>
+      <c r="K5" t="s">
         <v>22</v>
       </c>
-      <c r="H5">
-        <f>H9</f>
-        <v>1000</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5">
-        <f>IF(J5="S",2,1)*H5*E6</f>
-        <v>100000</v>
-      </c>
     </row>
     <row r="6" ht="15">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E6">
         <f>B5</f>
         <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H6">
         <f>H4*0.01</f>
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I6" t="str">
         <f>I4</f>
         <v>settimana</v>
       </c>
-      <c r="J6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6">
-        <f>IF(J6="S",2,1)*H6*E5</f>
-        <v>1000000000</v>
+      <c r="J6">
+        <f>H6*(E12+1+1+1+2+2+2)</f>
+        <v>10009000</v>
       </c>
     </row>
     <row r="7" ht="15">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>10000</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H7">
-        <f>4*E6</f>
+        <f>E9*4</f>
         <v>400</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7">
-        <f>IF(J7="S",2,1)*H7*E7</f>
-        <v>8000000</v>
+        <v>15</v>
+      </c>
+      <c r="J7">
+        <f>2*H7*4</f>
+        <v>3200</v>
       </c>
     </row>
     <row r="8" ht="15">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E8">
         <f>E7-E9</f>
         <v>9900</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H8">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8">
+        <f>2*H8</f>
+        <v>20</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" ht="15">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
         <v>1</v>
       </c>
-      <c r="I8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8">
-        <f>IF(J8="S",2,1)*H8*E15</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" ht="15">
       <c r="D9" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E9">
         <f>E6</f>
         <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H9">
-        <v>1000</v>
+        <f>E6*B2*B11</f>
+        <v>4000</v>
       </c>
       <c r="I9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" t="s">
         <v>15</v>
       </c>
-      <c r="K9">
-        <f>IF(J9="S",2,1)*H9</f>
-        <v>1000</v>
+      <c r="J9">
+        <f>H9</f>
+        <v>4000</v>
       </c>
     </row>
     <row r="10" ht="15">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E10">
         <f>E2</f>
@@ -953,26 +994,33 @@
       </c>
     </row>
     <row r="11" ht="15">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <f>B10</f>
+        <v>4</v>
+      </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E11">
         <f>E14+E12</f>
-        <v>100000000</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="12" ht="14.25">
       <c r="D12" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E12">
-        <f>B3*E2*E6/B2</f>
-        <v>1000000</v>
+        <f>B3*B2*E6</f>
+        <v>10000</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="D13" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E13">
         <f>E6</f>
@@ -981,29 +1029,25 @@
     </row>
     <row r="14" ht="14.25">
       <c r="D14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14">
-        <f>B3*E2*E8/B2</f>
-        <v>99000000</v>
+        <v>43</v>
+      </c>
+      <c r="E14" s="1">
+        <f>B2*B3*E8</f>
+        <v>990000</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" ht="14.25">
       <c r="D15" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E15">
         <v>100</v>
       </c>
     </row>
-    <row r="20" ht="14.25">
-      <c r="I20">
-        <v>4</v>
-      </c>
-    </row>
+    <row r="20" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
Aggiunti gli schemi sualla fase di progettazione concettuale e modifica delle operazioni (con relative frequenze e costi)
</commit_message>
<xml_diff>
--- a/doc/Volume dei dati.xlsx
+++ b/doc/Volume dei dati.xlsx
@@ -57,7 +57,7 @@
     <t xml:space="preserve">Carta di Credito</t>
   </si>
   <si>
-    <t xml:space="preserve">Visualizza lo stato delle aste dell'utente</t>
+    <t xml:space="preserve">Visualizza lo stato delle aste in corso</t>
   </si>
   <si>
     <t>settimana</t>
@@ -78,10 +78,7 @@
     <t>Controfferte</t>
   </si>
   <si>
-    <t xml:space="preserve">Visualizza nuove aste</t>
-  </si>
-  <si>
-    <t>NaN</t>
+    <t xml:space="preserve">Visualizza elenco oggetti all'asta</t>
   </si>
   <si>
     <t xml:space="preserve">Login a settimana</t>
@@ -93,22 +90,31 @@
     <t>Aste</t>
   </si>
   <si>
+    <t xml:space="preserve">Visualizza elenco oggetti aggiudicati</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1% delle offerte</t>
+  </si>
+  <si>
+    <t>Oggetto</t>
+  </si>
+  <si>
     <t xml:space="preserve">Controfferta Automatica</t>
   </si>
   <si>
-    <t xml:space="preserve">1% delle offerte</t>
-  </si>
-  <si>
-    <t>Oggetto</t>
+    <t xml:space="preserve">Numero di volte che un utente visualizza lo stato delle aste al giorno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oggetto Aggiudicato</t>
   </si>
   <si>
     <t xml:space="preserve">Inserisci oggetto</t>
   </si>
   <si>
-    <t xml:space="preserve">Numero di volte che un utente visualizza lo stato delle aste al giorno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oggetto Aggiudicato</t>
+    <t xml:space="preserve">Visualizza nuove aste per utente a login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oggetto all'asta</t>
   </si>
   <si>
     <t xml:space="preserve">Inserisci categoria</t>
@@ -117,19 +123,13 @@
     <t>anno</t>
   </si>
   <si>
-    <t xml:space="preserve">Visualizza nuove aste per utente a login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oggetto all'asta</t>
+    <t xml:space="preserve">Durata media asta</t>
+  </si>
+  <si>
+    <t>Possiede</t>
   </si>
   <si>
     <t>Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durata media asta</t>
-  </si>
-  <si>
-    <t>Possiede</t>
   </si>
   <si>
     <t xml:space="preserve">Login di un utente a settimana</t>
@@ -185,7 +185,8 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
@@ -697,7 +698,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -707,7 +708,7 @@
     <col bestFit="1" min="2" max="2" width="14.390625"/>
     <col bestFit="1" min="4" max="4" width="18.00390625"/>
     <col bestFit="1" customWidth="1" min="5" max="5" width="11.7109375"/>
-    <col bestFit="1" customWidth="1" min="7" max="7" width="33.87109375"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" width="45.79296875"/>
     <col bestFit="1" min="8" max="8" width="15.140625"/>
     <col customWidth="1" min="9" max="9" width="16.140625"/>
     <col customWidth="1" min="10" max="10" width="18.28125"/>
@@ -787,15 +788,15 @@
         <v>14</v>
       </c>
       <c r="H3">
-        <f>H9*B8</f>
+        <f>H10*B8</f>
         <v>40000</v>
       </c>
       <c r="I3" t="s">
         <v>15</v>
       </c>
       <c r="J3">
-        <f>H3*(1+B2*B4+B4+E14/E12*5)</f>
-        <v>20280000</v>
+        <f>H3*(E6+E12*2)</f>
+        <v>804000000</v>
       </c>
     </row>
     <row r="4" ht="15">
@@ -816,15 +817,15 @@
         <v>18</v>
       </c>
       <c r="H4">
-        <f>E12*B3</f>
-        <v>100000</v>
+        <f>B5*B3*B2*B4</f>
+        <v>10000</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>
       <c r="J4">
-        <f>2*H4*5</f>
-        <v>1000000</v>
+        <f>H4*(1+1+1)*2</f>
+        <v>60000</v>
       </c>
     </row>
     <row r="5" ht="15">
@@ -846,44 +847,45 @@
         <v>21</v>
       </c>
       <c r="H5">
-        <f>H9*B9*B11</f>
-        <v>16000</v>
+        <f>H10</f>
+        <v>4000</v>
       </c>
       <c r="I5" t="s">
         <v>15</v>
       </c>
-      <c r="J5" t="s">
-        <v>22</v>
+      <c r="J5">
+        <f>H5*(5*B5)</f>
+        <v>2000000</v>
       </c>
     </row>
     <row r="6" ht="15">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
       </c>
       <c r="E6">
         <f>B5</f>
         <v>100</v>
       </c>
-      <c r="G6" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6">
-        <f>H4*0.01</f>
-        <v>1000</v>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2">
+        <f>H10</f>
+        <v>4000</v>
       </c>
       <c r="I6" t="str">
         <f>I4</f>
         <v>settimana</v>
       </c>
       <c r="J6">
-        <f>H6*(E12+1+1+1+2+2+2)</f>
-        <v>10009000</v>
+        <f>H6*(E8*3)</f>
+        <v>118800000</v>
       </c>
     </row>
     <row r="7" ht="15">
@@ -891,103 +893,117 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
       </c>
       <c r="E7">
         <v>10000</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7">
-        <f>E9*4</f>
-        <v>400</v>
+        <f>H4*0.01</f>
+        <v>100</v>
       </c>
       <c r="I7" t="s">
         <v>15</v>
       </c>
       <c r="J7">
-        <f>2*H7*4</f>
-        <v>3200</v>
+        <f>H7*(2*4+3*B2*B3)</f>
+        <v>30800</v>
       </c>
     </row>
     <row r="8" ht="15">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <f>E7-E9</f>
         <v>9900</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8">
-        <v>10</v>
+        <f>E9*2</f>
+        <v>200</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="J8">
-        <f>2*H8</f>
-        <v>20</v>
-      </c>
-      <c r="K8" t="s">
-        <v>11</v>
+        <f>H8*2*5</f>
+        <v>2000</v>
       </c>
     </row>
     <row r="9" ht="15">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9">
         <f>E6</f>
         <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H9">
-        <f>E6*B2*B11</f>
-        <v>4000</v>
+        <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="J9">
-        <f>H9</f>
-        <v>4000</v>
+        <f>2*H9</f>
+        <v>20</v>
+      </c>
+      <c r="K9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" ht="15">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E10">
         <f>E2</f>
         <v>10000</v>
       </c>
+      <c r="G10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10">
+        <f>E6*B2*B11</f>
+        <v>4000</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10">
+        <f>H10</f>
+        <v>4000</v>
+      </c>
     </row>
     <row r="11" ht="15">
       <c r="A11" t="s">
@@ -1022,12 +1038,13 @@
         <f>E6</f>
         <v>100</v>
       </c>
+      <c r="G13"/>
     </row>
     <row r="14" ht="14.25">
       <c r="D14" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
         <f>B2*B3*E8</f>
         <v>990000</v>
       </c>
@@ -1043,6 +1060,8 @@
         <v>100</v>
       </c>
     </row>
+    <row r="16" ht="14.25"/>
+    <row r="17" ht="14.25"/>
     <row r="20" ht="14.25"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Refactoring operazioni e costi AGAIN
</commit_message>
<xml_diff>
--- a/doc/Volume dei dati.xlsx
+++ b/doc/Volume dei dati.xlsx
@@ -57,7 +57,7 @@
     <t xml:space="preserve">Carta di Credito</t>
   </si>
   <si>
-    <t xml:space="preserve">Visualizza lo stato delle aste in corso</t>
+    <t xml:space="preserve">Visualizza lo stato delle aste in corso di un utente</t>
   </si>
   <si>
     <t>settimana</t>
@@ -99,7 +99,7 @@
     <t>Oggetto</t>
   </si>
   <si>
-    <t xml:space="preserve">Controfferta Automatica</t>
+    <t xml:space="preserve">Imposta Controfferta</t>
   </si>
   <si>
     <t xml:space="preserve">Numero di volte che un utente visualizza lo stato delle aste al giorno</t>
@@ -138,7 +138,7 @@
     <t>Fa</t>
   </si>
   <si>
-    <t xml:space="preserve">Viene Fatta</t>
+    <t>Riceve</t>
   </si>
   <si>
     <t xml:space="preserve">Viene Messo</t>
@@ -159,9 +159,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -698,7 +698,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -795,8 +795,8 @@
         <v>15</v>
       </c>
       <c r="J3">
-        <f>H3*(E6+E12*2)</f>
-        <v>201000000</v>
+        <f>H3*(1+1+1+1+(B2*B3/2)*2)</f>
+        <v>1040000</v>
       </c>
     </row>
     <row r="4" ht="15">
@@ -810,22 +810,22 @@
         <v>17</v>
       </c>
       <c r="E4">
-        <f>E11</f>
+        <f>B2*B3*(E8+E9)</f>
         <v>1000000</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
       </c>
       <c r="H4">
-        <f>B5*B3*B2*B4</f>
+        <f>H10/B11*B3</f>
         <v>10000</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>
       <c r="J4">
-        <f>H4*(1+1+1)*2</f>
-        <v>60000</v>
+        <f>H4*((1+1+1)*2+1)</f>
+        <v>70000</v>
       </c>
     </row>
     <row r="5" ht="15">
@@ -847,15 +847,15 @@
         <v>21</v>
       </c>
       <c r="H5">
-        <f>H10/B11</f>
-        <v>1000</v>
+        <f>H10</f>
+        <v>4000</v>
       </c>
       <c r="I5" t="s">
         <v>15</v>
       </c>
       <c r="J5">
-        <f>H5*(5*B5)</f>
-        <v>500000</v>
+        <f>H5*((B5+E12*2+E9*4))</f>
+        <v>82000000</v>
       </c>
     </row>
     <row r="6" ht="15">
@@ -876,16 +876,16 @@
         <v>25</v>
       </c>
       <c r="H6" s="2">
-        <f>H10/B11</f>
-        <v>1000</v>
+        <f>100</f>
+        <v>100</v>
       </c>
       <c r="I6" t="str">
         <f>I4</f>
         <v>settimana</v>
       </c>
       <c r="J6">
-        <f>H6*(E8*3)</f>
-        <v>29700000</v>
+        <f>H6*((E14-E12)*2+E8*2)</f>
+        <v>199980000</v>
       </c>
     </row>
     <row r="7" ht="15">
@@ -905,15 +905,15 @@
         <v>28</v>
       </c>
       <c r="H7">
-        <f>H4*0.01</f>
-        <v>100</v>
+        <f>H4*0.1</f>
+        <v>1000</v>
       </c>
       <c r="I7" t="s">
         <v>15</v>
       </c>
       <c r="J7">
-        <f>H7*(2*4+3*B2*B3)</f>
-        <v>30800</v>
+        <f>H7*2*2</f>
+        <v>4000</v>
       </c>
     </row>
     <row r="8" ht="15">
@@ -1017,7 +1017,7 @@
         <v>40</v>
       </c>
       <c r="E11">
-        <f>E14+E12</f>
+        <f>E4</f>
         <v>1000000</v>
       </c>
     </row>
@@ -1044,8 +1044,8 @@
         <v>43</v>
       </c>
       <c r="E14" s="2">
-        <f>B2*B3*E8</f>
-        <v>990000</v>
+        <f>E4</f>
+        <v>1000000</v>
       </c>
       <c r="F14" t="s">
         <v>44</v>
@@ -1065,7 +1065,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>